<commit_message>
Modications and add Frontend
</commit_message>
<xml_diff>
--- a/Doc_Atividades/Acompanhar Minhas Tarefas1.xlsx
+++ b/Doc_Atividades/Acompanhar Minhas Tarefas1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matheus/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matheus/Documents/EloGroup/Doc_Atividades/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC33B1BD-0585-7E40-A4CD-AD83B54D3F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39505AA1-DE9C-3A4B-80A3-B52C4D3249C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7120" yWindow="2960" windowWidth="28780" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>LISTA DE TAREFAS</t>
   </si>
@@ -83,6 +83,12 @@
   <si>
     <t>(.Foi Criado  a Modelagem  do Formulario ainda falta A Lista de Usuarios )</t>
   </si>
+  <si>
+    <t>CRIAÇÃO DA API =&gt; BACKEND</t>
+  </si>
+  <si>
+    <t>FOI CRIADO A API REST PARA O ENVIO DE DADOS ATRAVES DO FORMULARIO</t>
+  </si>
 </sst>
 </file>
 
@@ -95,7 +101,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="&quot;Concluído&quot;;&quot;&quot;;&quot;&quot;"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,8 +267,13 @@
       <color rgb="FFB73FF6"/>
       <name val="Calibri (Corpo)"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFB73FF6"/>
+      <name val="Calibri (Corpo)"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,6 +462,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -637,7 +654,7 @@
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -679,6 +696,12 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="34" borderId="0" xfId="3" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="35" borderId="0" xfId="4" applyFont="1" applyFill="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" xfId="6" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -735,14 +758,6 @@
   </cellStyles>
   <dxfs count="19">
     <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -776,21 +791,6 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill>
           <fgColor indexed="64"/>
@@ -875,6 +875,21 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill>
           <fgColor indexed="64"/>
@@ -1014,6 +1029,14 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill>
@@ -1104,17 +1127,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tarefas" displayName="Tarefas" ref="B2:G6" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12">
-  <autoFilter ref="B2:G6" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tarefas" displayName="Tarefas" ref="B2:G7" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12">
+  <autoFilter ref="B2:G7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="MINHAS TAREFAS" totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="11" dataCellStyle="Texto de tabela"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="DATA DE INÍCIO" dataDxfId="8" totalsRowDxfId="9" dataCellStyle="Data"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="DATA DE ENTREGA" dataDxfId="6" totalsRowDxfId="7" dataCellStyle="Data"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="% CONCLUÍDO" dataDxfId="4" totalsRowDxfId="5" dataCellStyle="Porcentagem"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="CONCLUÍDO" dataDxfId="2" totalsRowDxfId="3" dataCellStyle="Concluído">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="MINHAS TAREFAS" totalsRowLabel="Total" dataDxfId="11" totalsRowDxfId="10" dataCellStyle="Texto de tabela"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="DATA DE INÍCIO" dataDxfId="9" totalsRowDxfId="8" dataCellStyle="Data"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="DATA DE ENTREGA" dataDxfId="7" totalsRowDxfId="6" dataCellStyle="Data"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="% CONCLUÍDO" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Porcentagem"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="CONCLUÍDO" dataDxfId="3" totalsRowDxfId="2" dataCellStyle="Concluído">
       <calculatedColumnFormula>--(Tarefas[[#This Row],[% CONCLUÍDO]]&gt;=1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ANOTAÇÕES" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="1" dataCellStyle="Texto de tabela"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="ANOTAÇÕES" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Texto de tabela"/>
   </tableColumns>
   <tableStyleInfo name="Lista de Tarefas" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1335,7 +1358,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="33" customHeight="1"/>
@@ -1459,7 +1482,7 @@
       <c r="D6" s="10">
         <v>43906</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="9">
         <v>0.8</v>
       </c>
       <c r="F6" s="13">
@@ -1472,12 +1495,25 @@
     </row>
     <row r="7" spans="1:7" ht="33" customHeight="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="B7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="10">
+        <v>43891</v>
+      </c>
+      <c r="D7" s="10">
+        <v>43906</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="F7" s="13">
+        <f>--(Tarefas[[#This Row],[% CONCLUÍDO]]&gt;=1)</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="33" customHeight="1">
       <c r="A8" s="2"/>
@@ -1537,7 +1573,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="542" yWindow="341" count="1">
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione um valor na lista suspensa. Ou digite um dos seguintes: 0%, 25%, 50%, 75% ou 100%" sqref="E3:E6" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione um valor na lista suspensa. Ou digite um dos seguintes: 0%, 25%, 50%, 75% ou 100%" sqref="E3:E7" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"0%,25%,50%,75%,100%"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1547,6 +1583,9 @@
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
+  <ignoredErrors>
+    <ignoredError sqref="E5:E6" listDataValidation="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -1571,6 +1610,23 @@
           <xm:sqref>E5:E6 E3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{C7880304-DF87-7047-80EA-D1CE2720B8A1}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:borderColor theme="5"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="50" id="{04B8B5C2-C7B5-4FE5-B018-764654046486}">
             <x14:iconSet custom="1">
               <x14:cfvo type="percent">
@@ -1588,23 +1644,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>F3</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{C7880304-DF87-7047-80EA-D1CE2720B8A1}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:borderColor theme="5"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="4" id="{C51A309D-0895-EB49-9978-9D42A2AE7570}">

</xml_diff>